<commit_message>
Menambah status masing-masing list pada file
</commit_message>
<xml_diff>
--- a/To do Learn.xlsx
+++ b/To do Learn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Memo\to do learn gl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA202F69-184C-4AA0-AF4A-A0A369E78B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC18D25C-0B51-4FFB-B853-BEF17942AE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B215BE47-CA93-4DC1-BD2C-F1899DCF624B}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>jurnal</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>tutup buku (bulanan dan tahunan)</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>perlu disesuaikan dgn kebutuhan</t>
+  </si>
+  <si>
+    <t>perlu disesuaikan dgn kebutuhan (untuk hapus data)</t>
   </si>
 </sst>
 </file>
@@ -401,42 +410,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1A905-D934-4408-A173-71C37E127467}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>